<commit_message>
images pour le web et mobile
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport journalier - Kamel.xlsx
+++ b/rapport journalier/Rapport journalier - Kamel.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelfilal\Desktop\mypetsitter\rapport journalier\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54dcebaf8a72f89b/Session 4 ETE ISI/Projet Final/mypetsitter/rapport journalier/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD6543A-AAE4-4C09-A6FE-36EDEDD05765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{4FD6543A-AAE4-4C09-A6FE-36EDEDD05765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC55B66E-EBA6-40E7-8B8F-EADA0312C912}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="32">
   <si>
     <t xml:space="preserve">DATE : </t>
   </si>
@@ -88,6 +88,39 @@
   </si>
   <si>
     <t>heritage de Activity pour le fragmentManager. Probleme resolue</t>
+  </si>
+  <si>
+    <t>Lundi</t>
+  </si>
+  <si>
+    <t>api fetcher</t>
+  </si>
+  <si>
+    <t>ras</t>
+  </si>
+  <si>
+    <t>connexion manager</t>
+  </si>
+  <si>
+    <t>ajouter animaux manager</t>
+  </si>
+  <si>
+    <t>revision des interfaces utilisateur jai refait tout les mockup pour enchainer pplus rapidement sur les vue</t>
+  </si>
+  <si>
+    <t>Recherche manager</t>
+  </si>
+  <si>
+    <t>Recherche Manager Maj des objets Gson car l'analyse a été modifier</t>
+  </si>
+  <si>
+    <t>vue xml pour aider michel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connexion fetch ver l'api </t>
+  </si>
+  <si>
+    <t>reflechir en meme temps au code de chaque fonctionalite dans l'application</t>
   </si>
 </sst>
 </file>
@@ -643,13 +676,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="14.42578125" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+    <col min="4" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -979,12 +1014,16 @@
       <c r="B43" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="2">
+        <v>44043</v>
+      </c>
       <c r="D43" s="17"/>
       <c r="E43" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F43" s="17"/>
+      <c r="F43" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G43" s="17"/>
       <c r="H43" s="4" t="s">
         <v>2</v>
@@ -996,6 +1035,12 @@
       <c r="B44" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
       <c r="J44" s="8"/>
     </row>
     <row r="45" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -1010,7 +1055,9 @@
       <c r="B47" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="C47" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -1046,12 +1093,16 @@
       <c r="B53" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="17"/>
+      <c r="C53" s="2">
+        <v>44046</v>
+      </c>
       <c r="D53" s="17"/>
       <c r="E53" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F53" s="17"/>
+      <c r="F53" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="G53" s="17"/>
       <c r="H53" s="4" t="s">
         <v>2</v>
@@ -1063,6 +1114,15 @@
       <c r="B54" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="C54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" t="s">
+        <v>22</v>
+      </c>
       <c r="J54" s="8"/>
     </row>
     <row r="55" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -1077,7 +1137,9 @@
       <c r="B57" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="11"/>
+      <c r="C57" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
@@ -1113,12 +1175,16 @@
       <c r="B63" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="17"/>
+      <c r="C63" s="2">
+        <v>44047</v>
+      </c>
       <c r="D63" s="17"/>
       <c r="E63" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F63" s="17"/>
+      <c r="F63" s="17" t="s">
+        <v>8</v>
+      </c>
       <c r="G63" s="17"/>
       <c r="H63" s="4" t="s">
         <v>2</v>
@@ -1130,6 +1196,12 @@
       <c r="B64" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="C64" t="s">
+        <v>29</v>
+      </c>
+      <c r="H64" t="s">
+        <v>22</v>
+      </c>
       <c r="J64" s="8"/>
     </row>
     <row r="65" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -1144,7 +1216,9 @@
       <c r="B67" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="11"/>
+      <c r="C67" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -1180,12 +1254,16 @@
       <c r="B73" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="17"/>
+      <c r="C73" s="2">
+        <v>44048</v>
+      </c>
       <c r="D73" s="17"/>
       <c r="E73" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F73" s="17"/>
+      <c r="F73" s="17" t="s">
+        <v>10</v>
+      </c>
       <c r="G73" s="17"/>
       <c r="H73" s="4" t="s">
         <v>2</v>
@@ -1197,6 +1275,9 @@
       <c r="B74" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="C74" t="s">
+        <v>28</v>
+      </c>
       <c r="J74" s="8"/>
     </row>
     <row r="75" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -1211,7 +1292,9 @@
       <c r="B77" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C77" s="11"/>
+      <c r="C77" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -1247,12 +1330,16 @@
       <c r="B83" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="17"/>
+      <c r="C83" s="2">
+        <v>44049</v>
+      </c>
       <c r="D83" s="17"/>
       <c r="E83" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F83" s="17"/>
+      <c r="F83" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="G83" s="17"/>
       <c r="H83" s="4" t="s">
         <v>2</v>
@@ -1264,6 +1351,9 @@
       <c r="B84" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="C84" t="s">
+        <v>26</v>
+      </c>
       <c r="J84" s="8"/>
     </row>
     <row r="85" spans="2:10" ht="14.25" x14ac:dyDescent="0.2">
@@ -1278,7 +1368,9 @@
       <c r="B87" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C87" s="11"/>
+      <c r="C87" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
@@ -1314,12 +1406,16 @@
       <c r="B93" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C93" s="17"/>
+      <c r="C93" s="2">
+        <v>44050</v>
+      </c>
       <c r="D93" s="17"/>
       <c r="E93" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F93" s="17"/>
+      <c r="F93" s="17" t="s">
+        <v>17</v>
+      </c>
       <c r="G93" s="17"/>
       <c r="H93" s="4" t="s">
         <v>2</v>
@@ -1330,6 +1426,9 @@
     <row r="94" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="20" t="s">
         <v>3</v>
+      </c>
+      <c r="C94" t="s">
+        <v>30</v>
       </c>
       <c r="J94" s="8"/>
     </row>

</xml_diff>